<commit_message>
BOM Updated with printed Parts
</commit_message>
<xml_diff>
--- a/Bill Of Materials/Printer Kitten BOM (Known Not Accurate, missing and incorrect parts).xlsx
+++ b/Bill Of Materials/Printer Kitten BOM (Known Not Accurate, missing and incorrect parts).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5370"/>
   </bookViews>
   <sheets>
     <sheet name="Kitten with Heated Bed" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="149">
   <si>
     <t>robotdigg</t>
   </si>
@@ -59,9 +59,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Discounted Parts Cost</t>
-  </si>
-  <si>
     <t>Number Of Parts</t>
   </si>
   <si>
@@ -365,19 +362,109 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>Recommended Settings with a .4mm Nozzle</t>
-  </si>
-  <si>
-    <t>Shell Thickness</t>
-  </si>
-  <si>
-    <t>Bottom/Top Thickness</t>
-  </si>
-  <si>
-    <t>Layer Height</t>
-  </si>
-  <si>
-    <t>Infill Percentage</t>
+    <t>Printed Part, Corner, Upper Front Right</t>
+  </si>
+  <si>
+    <t>Printed Part, Corner, Upper Front Left</t>
+  </si>
+  <si>
+    <t>Printed Part, Corner, Upper Back Right</t>
+  </si>
+  <si>
+    <t>Printed Part, X&amp;Y End</t>
+  </si>
+  <si>
+    <t>Printed Part, X&amp;Y End Belt Clamp 1</t>
+  </si>
+  <si>
+    <t>Printed Part, X&amp;Y End Belt Clamp 2</t>
+  </si>
+  <si>
+    <t>Printed Part, X&amp;Y End Belt Clamp 3</t>
+  </si>
+  <si>
+    <t>Printed Part, Print Head Body</t>
+  </si>
+  <si>
+    <t>Printed Part, Print Head Clamp</t>
+  </si>
+  <si>
+    <t>Printed Part, Bondtech Housing Front 1.75</t>
+  </si>
+  <si>
+    <t>Printed Part, Bondtech Housing Rear</t>
+  </si>
+  <si>
+    <t>Printed Part, Y Motor Mount</t>
+  </si>
+  <si>
+    <t>Printed Part, Z Motor Mount</t>
+  </si>
+  <si>
+    <t>Printed Part, Lower Rod Mount</t>
+  </si>
+  <si>
+    <t>Printed Part, X&amp;Y Belt Guide</t>
+  </si>
+  <si>
+    <t>Printed Part, X&amp;Y Spacer</t>
+  </si>
+  <si>
+    <t>Printed Part, Upper Rod Mount</t>
+  </si>
+  <si>
+    <t>Printed Part, Z End Stop Mount</t>
+  </si>
+  <si>
+    <t>Printed Part, Z End Stop Magnet Mount</t>
+  </si>
+  <si>
+    <t>Printed Part, Z Adjustment Nut</t>
+  </si>
+  <si>
+    <t>Printed Part, Spool Holder Part1</t>
+  </si>
+  <si>
+    <t>Printed Part, BondTech Clamp1</t>
+  </si>
+  <si>
+    <t>Printed Part, BondTech Clamp2</t>
+  </si>
+  <si>
+    <t>Printed Part, Spool Holder Part2</t>
+  </si>
+  <si>
+    <t>Printed Part, Spool Holder Part3</t>
+  </si>
+  <si>
+    <t>Printed Part, Spool Holder Part4</t>
+  </si>
+  <si>
+    <t>Printed Part, IO Mount</t>
+  </si>
+  <si>
+    <t>total Printed parts</t>
+  </si>
+  <si>
+    <t>Printed Part, Rambo Mini Mount 1</t>
+  </si>
+  <si>
+    <t>Printed Part, Rambo Mini Mount 2</t>
+  </si>
+  <si>
+    <t>Printed Part, LCD Mount 1</t>
+  </si>
+  <si>
+    <t>Printed Part, LCD Mount 2</t>
+  </si>
+  <si>
+    <t>Printed Part, LCD Mount 3</t>
+  </si>
+  <si>
+    <t>Printed Part, LCD Mount 4</t>
+  </si>
+  <si>
+    <t>Parts Cost</t>
   </si>
 </sst>
 </file>
@@ -755,7 +842,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -765,13 +852,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
@@ -788,7 +875,7 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="4" customFormat="1">
@@ -808,13 +895,13 @@
     </row>
     <row r="4" spans="1:17" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>4</v>
@@ -826,18 +913,18 @@
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="C5" s="1">
         <v>6.8</v>
@@ -856,7 +943,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -869,10 +956,10 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="C6" s="1">
         <v>32.5</v>
@@ -901,10 +988,10 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="C7" s="1">
         <v>5</v>
@@ -923,7 +1010,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -939,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1">
         <v>9</v>
@@ -958,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -971,10 +1058,10 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="C9" s="1">
         <v>1.8</v>
@@ -1003,10 +1090,10 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="C10" s="1">
         <v>1.8</v>
@@ -1035,10 +1122,10 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1">
         <v>28</v>
@@ -1067,10 +1154,10 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1">
         <v>1.85</v>
@@ -1102,7 +1189,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1">
         <v>1.8</v>
@@ -1131,10 +1218,10 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C14" s="1">
         <v>15.8</v>
@@ -1163,7 +1250,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>12</v>
@@ -1185,7 +1272,7 @@
         <v>9</v>
       </c>
       <c r="H15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1198,7 +1285,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>12</v>
@@ -1220,7 +1307,7 @@
         <v>9</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1233,7 +1320,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>12</v>
@@ -1255,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="H17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1268,7 +1355,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="1">
         <v>24.99</v>
@@ -1287,7 +1374,7 @@
         <v>9</v>
       </c>
       <c r="H18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1300,7 +1387,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" s="1">
         <v>29</v>
@@ -1329,10 +1416,10 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="C20" s="2">
         <v>120</v>
@@ -1348,10 +1435,10 @@
         <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1364,10 +1451,10 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="1">
         <v>8.44</v>
@@ -1396,10 +1483,10 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="C22" s="1">
         <v>6.6</v>
@@ -1428,10 +1515,10 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="C23" s="1">
         <v>8.3699999999999992</v>
@@ -1460,10 +1547,10 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="1">
         <v>13.35</v>
@@ -1492,10 +1579,10 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="C25" s="1">
         <v>9.82</v>
@@ -1524,10 +1611,10 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="C26" s="1">
         <v>8.2799999999999994</v>
@@ -1556,10 +1643,10 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="C27" s="1">
         <v>2.64</v>
@@ -1588,10 +1675,10 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="C28" s="1">
         <v>2.64</v>
@@ -1620,10 +1707,10 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="1">
         <v>8.81</v>
@@ -1652,10 +1739,10 @@
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" s="1">
         <v>12.3</v>
@@ -1684,10 +1771,10 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1">
         <v>14.4</v>
@@ -1716,10 +1803,10 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="C32" s="1">
         <v>5.0199999999999996</v>
@@ -1748,10 +1835,10 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="C33" s="1">
         <v>7.07</v>
@@ -1780,7 +1867,7 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>11</v>
@@ -1812,10 +1899,10 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
         <v>71</v>
-      </c>
-      <c r="B35" t="s">
-        <v>72</v>
       </c>
       <c r="C35" s="1">
         <v>3.87</v>
@@ -1844,10 +1931,10 @@
     </row>
     <row r="36" spans="1:17">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C36" s="1">
         <v>6</v>
@@ -1876,10 +1963,10 @@
     </row>
     <row r="37" spans="1:17">
       <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="C37" s="1">
         <v>2.52</v>
@@ -1898,7 +1985,7 @@
         <v>10</v>
       </c>
       <c r="H37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -1911,10 +1998,10 @@
     </row>
     <row r="38" spans="1:17">
       <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
         <v>81</v>
-      </c>
-      <c r="B38" t="s">
-        <v>82</v>
       </c>
       <c r="C38" s="1">
         <v>10.35</v>
@@ -1943,10 +2030,10 @@
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="12">
         <v>13.24</v>
@@ -1965,7 +2052,7 @@
         <v>10</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -1978,10 +2065,10 @@
     </row>
     <row r="40" spans="1:17">
       <c r="A40" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" s="1">
         <v>8.39</v>
@@ -2000,7 +2087,7 @@
         <v>10</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -2013,10 +2100,10 @@
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
         <v>89</v>
-      </c>
-      <c r="B41" t="s">
-        <v>90</v>
       </c>
       <c r="C41" s="1">
         <v>1.25</v>
@@ -2045,7 +2132,7 @@
     </row>
     <row r="42" spans="1:17">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C42" s="1">
         <v>40</v>
@@ -2061,10 +2148,10 @@
         <v>3</v>
       </c>
       <c r="G42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -2077,7 +2164,7 @@
     </row>
     <row r="43" spans="1:17">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" s="1">
         <v>60</v>
@@ -2093,10 +2180,10 @@
         <v>3</v>
       </c>
       <c r="G43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
@@ -2109,7 +2196,7 @@
     </row>
     <row r="44" spans="1:17">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="12">
         <v>7.9</v>
@@ -2125,10 +2212,10 @@
         <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
@@ -2141,7 +2228,7 @@
     </row>
     <row r="45" spans="1:17">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" s="12">
         <v>1.7</v>
@@ -2157,10 +2244,10 @@
         <v>2</v>
       </c>
       <c r="G45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
@@ -2173,7 +2260,7 @@
     </row>
     <row r="46" spans="1:17">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C46" s="12">
         <v>10</v>
@@ -2189,10 +2276,10 @@
         <v>2</v>
       </c>
       <c r="G46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
@@ -2205,10 +2292,10 @@
     </row>
     <row r="47" spans="1:17">
       <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
         <v>99</v>
-      </c>
-      <c r="B47" t="s">
-        <v>100</v>
       </c>
       <c r="C47" s="1">
         <v>0.6</v>
@@ -2224,7 +2311,7 @@
         <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -2245,10 +2332,10 @@
     <row r="49" spans="2:7">
       <c r="C49" s="12"/>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="2:7">
@@ -2285,14 +2372,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -2301,40 +2389,294 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="D2" s="16" t="s">
-        <v>115</v>
-      </c>
+      <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
         <v>113</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
         <v>114</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
         <v>118</v>
       </c>
-      <c r="E3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="D4">
-        <v>0.12</v>
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38">
+        <f>SUM(B4:B36)</f>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>